<commit_message>
refresh dataset + rebuild
</commit_message>
<xml_diff>
--- a/docs/data/eruptions_recent.xlsx
+++ b/docs/data/eruptions_recent.xlsx
@@ -32,7 +32,7 @@
     <t>vei</t>
   </si>
   <si>
-    <t>Kilauea</t>
+    <t>Kīlauea</t>
   </si>
   <si>
     <t>Atka Volcanic Complex</t>
@@ -404,10 +404,10 @@
         <v>44341.0</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>45495.0</v>
+        <v>45496.0</v>
       </c>
       <c r="D13" t="n">
-        <v>1154.0</v>
+        <v>1155.0</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>

</xml_diff>